<commit_message>
Slight tweaks to Baylor's Excel file to improve parsing of compensation controls.
</commit_message>
<xml_diff>
--- a/Baylor.xlsx
+++ b/Baylor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Comp controls" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>all</t>
   </si>
   <si>
-    <t>CD197 PE</t>
-  </si>
-  <si>
     <t>Min MFI</t>
   </si>
   <si>
@@ -391,13 +388,16 @@
     <t>CD45RA:PE-Cy7</t>
   </si>
   <si>
-    <t>CD4:PerCP-Cy5.5</t>
-  </si>
-  <si>
     <t>LIVE GREEN:FITC</t>
   </si>
   <si>
     <t>PLEASE FILL IN THE YELLOW SHADED CELLS:</t>
+  </si>
+  <si>
+    <t>CD197:PE</t>
+  </si>
+  <si>
+    <t>CD4:PerCP-Cy5-5</t>
   </si>
 </sst>
 </file>
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1173,7 +1173,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1193,10 +1193,10 @@
     </row>
     <row r="3" spans="1:8" ht="16" thickBot="1">
       <c r="A3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>16</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>0</v>
@@ -1205,27 +1205,27 @@
         <v>1</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>6</v>
-      </c>
       <c r="H3" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>2</v>
@@ -1245,13 +1245,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>2</v>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>2</v>
@@ -1297,42 +1297,42 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3">
         <v>27000</v>
@@ -1349,94 +1349,94 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3">
         <v>22500</v>
@@ -1453,94 +1453,94 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="F13" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="F15" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="3">
         <v>22500</v>
@@ -1557,39 +1557,39 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>2</v>
@@ -1609,13 +1609,13 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>2</v>
@@ -1649,7 +1649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1663,36 +1663,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1"/>
     <row r="3" spans="1:5" ht="16" thickBot="1">
       <c r="A3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="19" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1703,13 +1703,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1720,13 +1720,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1737,13 +1737,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1754,13 +1754,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1771,13 +1771,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1788,13 +1788,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1805,13 +1805,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1822,13 +1822,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1839,13 +1839,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1856,13 +1856,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1873,13 +1873,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -1890,13 +1890,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1907,13 +1907,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1941,13 +1941,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1958,13 +1958,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1975,13 +1975,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1992,13 +1992,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2009,13 +2009,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -2026,13 +2026,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -2043,13 +2043,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2060,13 +2060,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -2077,13 +2077,13 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -2094,13 +2094,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2111,13 +2111,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -2128,13 +2128,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -2145,13 +2145,13 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -2179,13 +2179,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -2196,13 +2196,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -2213,13 +2213,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -2230,13 +2230,13 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -2247,13 +2247,13 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -2264,13 +2264,13 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -2281,13 +2281,13 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -2298,13 +2298,13 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -2315,13 +2315,13 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -2332,13 +2332,13 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -2349,13 +2349,13 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2366,13 +2366,13 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -2383,13 +2383,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -2417,13 +2417,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -2434,13 +2434,13 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -2477,578 +2477,578 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B62" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B63" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B71" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -3077,7 +3077,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -3085,47 +3085,47 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pregates compensation controls in a smarter way before constructing spillover matrix. Also, manually updated Excel files for each center to improve parsing.
</commit_message>
<xml_diff>
--- a/Baylor.xlsx
+++ b/Baylor.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="141">
   <si>
     <t>Marker</t>
   </si>
@@ -349,55 +349,103 @@
     <t>Comment_GO</t>
   </si>
   <si>
-    <t>HLA-DR:V500</t>
-  </si>
-  <si>
-    <t>CD3:V450</t>
-  </si>
-  <si>
-    <t>CD3+19+20:APC-H7</t>
-  </si>
-  <si>
-    <t>CD20:APC-H7</t>
-  </si>
-  <si>
-    <t>CD45RO:APC-H7</t>
-  </si>
-  <si>
-    <t>CD8:APC-H7</t>
-  </si>
-  <si>
-    <t>CD127:Alexa 647</t>
-  </si>
-  <si>
-    <t>CD38:APC</t>
-  </si>
-  <si>
-    <t>CD196:PE-Cy7</t>
-  </si>
-  <si>
-    <t>CD11c:PE-Cy7</t>
-  </si>
-  <si>
-    <t>CD27:PE-Cy7</t>
-  </si>
-  <si>
-    <t>CD194:PE-Cy7</t>
-  </si>
-  <si>
-    <t>CD45RA:PE-Cy7</t>
-  </si>
-  <si>
-    <t>LIVE GREEN:FITC</t>
-  </si>
-  <si>
     <t>PLEASE FILL IN THE YELLOW SHADED CELLS:</t>
   </si>
   <si>
-    <t>CD197:PE</t>
-  </si>
-  <si>
-    <t>CD4:PerCP-Cy5-5</t>
+    <t>LIVE GREEN:FITC-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD45RA PE-Cy7-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD45RA:PE-Cy7-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD194 PE-Cy7-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD194:PE-Cy7-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD27 PE-Cy7-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD27:PE-Cy7-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD11c PE-Cy7-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD11c:PE-Cy7-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD196 PE-Cy7-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD196:PE-Cy7-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_LIVE GREEN FITC-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD197:PE-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD197 PE-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD4 PerCP-Cy5-5-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD4:PerCP-Cy5-5-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD3 V450-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>Compensation Controls_HLA-DR V500-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD3:V450-A</t>
+  </si>
+  <si>
+    <t>HLA-DR:V500-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD8 APC-H7-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD8:APC-H7-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD45RO APC-H7-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD45RO:APC-H7-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD20 APC-H7-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD20:APC-H7-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD3+19+20 APC-H7-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>CD3+19+20:APC-H7-A</t>
+  </si>
+  <si>
+    <t>CD38:APC-A</t>
+  </si>
+  <si>
+    <t>CD127:APC-A</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD38 APC-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD127 APC-A Stained Control.fcs</t>
   </si>
 </sst>
 </file>
@@ -1159,13 +1207,14 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="7" width="10.33203125" customWidth="1"/>
     <col min="8" max="8" width="22.5" customWidth="1"/>
@@ -1173,7 +1222,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="22" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1219,13 +1268,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="17" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>91</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>2</v>
@@ -1245,13 +1294,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>2</v>
@@ -1271,7 +1320,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>91</v>
@@ -1297,13 +1346,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>6</v>
@@ -1323,13 +1372,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>7</v>
@@ -1349,13 +1398,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="5" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>9</v>
@@ -1375,7 +1424,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>91</v>
@@ -1401,13 +1450,13 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>11</v>
@@ -1427,13 +1476,13 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
@@ -1453,13 +1502,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>7</v>
@@ -1479,13 +1528,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>13</v>
@@ -1505,13 +1554,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>7</v>
@@ -1531,13 +1580,13 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>9</v>
@@ -1557,13 +1606,13 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>10</v>
@@ -1583,13 +1632,13 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="5" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>2</v>
@@ -1609,13 +1658,13 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="11" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>91</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>2</v>
@@ -1663,7 +1712,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="22" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1"/>

</xml_diff>